<commit_message>
Major update vertical movement analyses. Timezone adjusted for date-time recorded by tag.
</commit_message>
<xml_diff>
--- a/Scripts_Vert/Outputs/summary.xlsx
+++ b/Scripts_Vert/Outputs/summary.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denisse\Documents\Manuscripts\miniPAT_SatTags\VerticalMovements\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33D2D2C-D198-4025-96BC-FD5CD113E33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0A2B27-269E-43B1-8033-483E28123A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="PERMANOVA_MinDepth" sheetId="3" r:id="rId3"/>
+    <sheet name="PERMANOVA_MaxDepth" sheetId="4" r:id="rId4"/>
+    <sheet name="PERMANOVA_MeanTemp" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="105">
   <si>
     <t>Measurements</t>
   </si>
@@ -252,13 +255,97 @@
   </si>
   <si>
     <t>91.5 (0.5 - 979)</t>
+  </si>
+  <si>
+    <t>Permutation: free</t>
+  </si>
+  <si>
+    <t>Number of permutations: 999</t>
+  </si>
+  <si>
+    <t>Terms added sequentially (first to last)</t>
+  </si>
+  <si>
+    <t>Diel</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>Df</t>
+  </si>
+  <si>
+    <t>SumsOfSqs</t>
+  </si>
+  <si>
+    <t>MeanSqs</t>
+  </si>
+  <si>
+    <t>F.Model</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Pr(&gt;F)</t>
+  </si>
+  <si>
+    <t>diel</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>ptt</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Diel*ptt*month</t>
+  </si>
+  <si>
+    <t>diel:ptt</t>
+  </si>
+  <si>
+    <t>diel:month</t>
+  </si>
+  <si>
+    <t>ptt:month</t>
+  </si>
+  <si>
+    <t>diel:ptt:month</t>
+  </si>
+  <si>
+    <t>Diel*month</t>
+  </si>
+  <si>
+    <t>Diel*ptt</t>
+  </si>
+  <si>
+    <t>ptt*month</t>
+  </si>
+  <si>
+    <t>ermutation: free</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,8 +493,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,6 +690,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -777,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -787,6 +904,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,19 +920,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1225,7 +1364,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -1266,7 +1405,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1444,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1344,7 +1483,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="A5" s="16"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +1522,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
+      <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1561,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
+      <c r="A7" s="16"/>
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1600,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1502,7 +1641,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1680,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1580,7 +1719,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1758,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1658,7 +1797,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1697,7 +1836,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1738,7 +1877,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
@@ -1777,7 +1916,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1816,7 +1955,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1855,7 +1994,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
@@ -1894,7 +2033,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="10"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1933,7 +2072,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1974,7 +2113,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
@@ -2013,7 +2152,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="10"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
@@ -2052,7 +2191,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="10"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
@@ -2091,7 +2230,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
@@ -2130,7 +2269,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
@@ -2169,7 +2308,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2210,7 +2349,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
@@ -2249,7 +2388,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="10"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
@@ -2288,7 +2427,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
@@ -2327,7 +2466,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2505,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="3" t="s">
         <v>7</v>
       </c>
@@ -2405,7 +2544,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2446,7 +2585,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="10"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
@@ -2485,7 +2624,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
@@ -2524,7 +2663,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
@@ -2563,7 +2702,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2602,7 +2741,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="10"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2641,7 +2780,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2682,7 +2821,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="3" t="s">
         <v>3</v>
       </c>
@@ -2721,7 +2860,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
+      <c r="A40" s="14"/>
       <c r="B40" s="3" t="s">
         <v>4</v>
       </c>
@@ -2760,7 +2899,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="10"/>
+      <c r="A41" s="14"/>
       <c r="B41" s="3" t="s">
         <v>5</v>
       </c>
@@ -2799,7 +2938,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="3" t="s">
         <v>6</v>
       </c>
@@ -2838,7 +2977,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="10"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2877,7 +3016,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2918,7 +3057,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +3096,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="10"/>
+      <c r="A46" s="14"/>
       <c r="B46" s="3" t="s">
         <v>4</v>
       </c>
@@ -2996,7 +3135,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="10"/>
+      <c r="A47" s="14"/>
       <c r="B47" s="3" t="s">
         <v>5</v>
       </c>
@@ -3035,7 +3174,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="10"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="3" t="s">
         <v>6</v>
       </c>
@@ -3074,7 +3213,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="11"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
@@ -3135,184 +3274,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A26282-6A4B-4AE8-B871-68E7B1E374FF}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="14"/>
+    <col min="1" max="1" width="6.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.90625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="15.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13">
+      <c r="C1" s="9">
         <v>157560</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="9">
         <v>157561</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="9">
         <v>157562</v>
       </c>
-      <c r="F1" s="13">
+      <c r="F1" s="9">
         <v>157566</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G1" s="9">
         <v>157567</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="9">
         <v>157568</v>
       </c>
-      <c r="I1" s="13">
+      <c r="I1" s="9">
         <v>174048</v>
       </c>
-      <c r="J1" s="13">
+      <c r="J1" s="9">
         <v>174049</v>
       </c>
-      <c r="K1" s="13">
+      <c r="K1" s="9">
         <v>174050</v>
       </c>
-      <c r="L1" s="13">
+      <c r="L1" s="9">
         <v>174051</v>
       </c>
-      <c r="M1" s="13">
+      <c r="M1" s="9">
         <v>178974</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="14" t="s">
+      <c r="I2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="D3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="D4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="17" t="s">
+      <c r="H4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3320,81 +3459,81 @@
       <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="D5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="19" t="s">
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="17" t="s">
+      <c r="I6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3402,81 +3541,81 @@
       <c r="A7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="19" t="s">
+      <c r="I7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="17" t="s">
+      <c r="C8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="17" t="s">
+      <c r="H8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3484,81 +3623,81 @@
       <c r="A9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="C9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="17" t="s">
+      <c r="C10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="17" t="s">
+      <c r="H10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3566,81 +3705,81 @@
       <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="19" t="s">
+      <c r="C11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="19" t="s">
+      <c r="H11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="17" t="s">
+      <c r="C12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3648,81 +3787,81 @@
       <c r="A13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="19" t="s">
+      <c r="C13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L13" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="M13" s="19" t="s">
+      <c r="M13" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="17" t="s">
+      <c r="C14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3730,81 +3869,81 @@
       <c r="A15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="19" t="s">
+      <c r="C15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="17" t="s">
+      <c r="C16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3812,57 +3951,57 @@
       <c r="A17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="19" t="s">
+      <c r="C17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="M17" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3878,4 +4017,1774 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FB3C07-509B-4E9C-9FF1-781FCA8304C0}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1707</v>
+      </c>
+      <c r="D8">
+        <v>1707</v>
+      </c>
+      <c r="E8">
+        <v>1.0773999999999999</v>
+      </c>
+      <c r="F8">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="G8">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>13973</v>
+      </c>
+      <c r="L8">
+        <v>1397.3</v>
+      </c>
+      <c r="M8">
+        <v>0.88107000000000002</v>
+      </c>
+      <c r="N8">
+        <v>6.3099999999999996E-3</v>
+      </c>
+      <c r="O8">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>1396</v>
+      </c>
+      <c r="C9">
+        <v>2211909</v>
+      </c>
+      <c r="D9">
+        <v>1584.5</v>
+      </c>
+      <c r="F9">
+        <v>0.99922999999999995</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9">
+        <v>1387</v>
+      </c>
+      <c r="K9">
+        <v>2199643</v>
+      </c>
+      <c r="L9">
+        <v>1585.9</v>
+      </c>
+      <c r="N9">
+        <v>0.99368999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>1397</v>
+      </c>
+      <c r="C10">
+        <v>2213616</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10">
+        <v>1397</v>
+      </c>
+      <c r="K10">
+        <v>2213616</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="21"/>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19" t="s">
+        <v>87</v>
+      </c>
+      <c r="N19" t="s">
+        <v>88</v>
+      </c>
+      <c r="O19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>4.04</v>
+      </c>
+      <c r="E20">
+        <v>2.5466E-3</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1643</v>
+      </c>
+      <c r="L20">
+        <v>1642.8</v>
+      </c>
+      <c r="M20">
+        <v>1.0367999999999999</v>
+      </c>
+      <c r="N20">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="O20">
+        <v>0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21">
+        <v>1396</v>
+      </c>
+      <c r="C21">
+        <v>2213612</v>
+      </c>
+      <c r="D21">
+        <v>1585.68</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21">
+        <v>1396</v>
+      </c>
+      <c r="K21">
+        <v>2211973</v>
+      </c>
+      <c r="L21">
+        <v>1584.5</v>
+      </c>
+      <c r="N21">
+        <v>0.99926000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22">
+        <v>1397</v>
+      </c>
+      <c r="C22">
+        <v>2213616</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22">
+        <v>1397</v>
+      </c>
+      <c r="K22">
+        <v>2213616</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026B9B64-649A-4C7B-8F7F-8F18A560B383}">
+  <dimension ref="A1:W40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="J7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1637096</v>
+      </c>
+      <c r="D8">
+        <v>1637096</v>
+      </c>
+      <c r="E8">
+        <v>16.643000000000001</v>
+      </c>
+      <c r="F8">
+        <v>1.1780000000000001E-2</v>
+      </c>
+      <c r="G8" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>11855637</v>
+      </c>
+      <c r="L8">
+        <v>1185564</v>
+      </c>
+      <c r="M8">
+        <v>12.938000000000001</v>
+      </c>
+      <c r="N8">
+        <v>8.5319999999999993E-2</v>
+      </c>
+      <c r="O8" s="23">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>1396</v>
+      </c>
+      <c r="C9">
+        <v>137319244</v>
+      </c>
+      <c r="D9">
+        <v>98366</v>
+      </c>
+      <c r="F9">
+        <v>0.98821999999999999</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9">
+        <v>1387</v>
+      </c>
+      <c r="K9">
+        <v>127100703</v>
+      </c>
+      <c r="L9">
+        <v>91637</v>
+      </c>
+      <c r="N9">
+        <v>0.91468000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>1397</v>
+      </c>
+      <c r="C10">
+        <v>138956340</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10">
+        <v>1397</v>
+      </c>
+      <c r="K10">
+        <v>138956340</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q13" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q14" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q15" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="Q16" s="21"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q17" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="Q18" s="21"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19" t="s">
+        <v>87</v>
+      </c>
+      <c r="N19" t="s">
+        <v>88</v>
+      </c>
+      <c r="O19" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q19" s="20"/>
+      <c r="R19" t="s">
+        <v>84</v>
+      </c>
+      <c r="S19" t="s">
+        <v>85</v>
+      </c>
+      <c r="T19" t="s">
+        <v>86</v>
+      </c>
+      <c r="U19" t="s">
+        <v>87</v>
+      </c>
+      <c r="V19" t="s">
+        <v>88</v>
+      </c>
+      <c r="W19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>18866</v>
+      </c>
+      <c r="D20">
+        <v>18866</v>
+      </c>
+      <c r="E20">
+        <v>0.18956000000000001</v>
+      </c>
+      <c r="F20">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="G20">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1457914</v>
+      </c>
+      <c r="L20">
+        <v>1457914</v>
+      </c>
+      <c r="M20">
+        <v>14.802</v>
+      </c>
+      <c r="N20">
+        <v>1.0489999999999999E-2</v>
+      </c>
+      <c r="O20" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="Q20" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1637096</v>
+      </c>
+      <c r="T20">
+        <v>1637096</v>
+      </c>
+      <c r="U20">
+        <v>18.029499999999999</v>
+      </c>
+      <c r="V20">
+        <v>1.1780000000000001E-2</v>
+      </c>
+      <c r="W20" s="23">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21">
+        <v>1396</v>
+      </c>
+      <c r="C21">
+        <v>138937474</v>
+      </c>
+      <c r="D21">
+        <v>99525</v>
+      </c>
+      <c r="F21">
+        <v>0.99985999999999997</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21">
+        <v>1396</v>
+      </c>
+      <c r="K21">
+        <v>137498426</v>
+      </c>
+      <c r="L21">
+        <v>98495</v>
+      </c>
+      <c r="N21">
+        <v>0.98951</v>
+      </c>
+      <c r="Q21" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="R21">
+        <v>10</v>
+      </c>
+      <c r="S21">
+        <v>11740124</v>
+      </c>
+      <c r="T21">
+        <v>1174012</v>
+      </c>
+      <c r="U21">
+        <v>12.929500000000001</v>
+      </c>
+      <c r="V21">
+        <v>8.4489999999999996E-2</v>
+      </c>
+      <c r="W21" s="23">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22">
+        <v>1397</v>
+      </c>
+      <c r="C22">
+        <v>138956340</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22">
+        <v>1397</v>
+      </c>
+      <c r="K22">
+        <v>138956340</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="R22">
+        <v>10</v>
+      </c>
+      <c r="S22">
+        <v>637017</v>
+      </c>
+      <c r="T22">
+        <v>63702</v>
+      </c>
+      <c r="U22">
+        <v>0.7016</v>
+      </c>
+      <c r="V22">
+        <v>4.5799999999999999E-3</v>
+      </c>
+      <c r="W22">
+        <v>0.72099999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Q23" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="R23">
+        <v>1376</v>
+      </c>
+      <c r="S23">
+        <v>124942103</v>
+      </c>
+      <c r="T23">
+        <v>90801</v>
+      </c>
+      <c r="V23">
+        <v>0.89915</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Q24" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="R24">
+        <v>1397</v>
+      </c>
+      <c r="S24">
+        <v>138956340</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A25" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q26" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q27" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="Q28" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q29" s="21"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="Q30" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A31" s="20"/>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="20"/>
+      <c r="J31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" t="s">
+        <v>85</v>
+      </c>
+      <c r="L31" t="s">
+        <v>86</v>
+      </c>
+      <c r="M31" t="s">
+        <v>87</v>
+      </c>
+      <c r="N31" t="s">
+        <v>88</v>
+      </c>
+      <c r="O31" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q31" s="21"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1637096</v>
+      </c>
+      <c r="D32">
+        <v>1637096</v>
+      </c>
+      <c r="E32">
+        <v>18.931000000000001</v>
+      </c>
+      <c r="F32">
+        <v>1.1780000000000001E-2</v>
+      </c>
+      <c r="G32" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1637096</v>
+      </c>
+      <c r="L32">
+        <v>1637096</v>
+      </c>
+      <c r="M32">
+        <v>16.796900000000001</v>
+      </c>
+      <c r="N32">
+        <v>1.1780000000000001E-2</v>
+      </c>
+      <c r="O32" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="Q32" s="20"/>
+      <c r="R32" t="s">
+        <v>84</v>
+      </c>
+      <c r="S32" t="s">
+        <v>85</v>
+      </c>
+      <c r="T32" t="s">
+        <v>86</v>
+      </c>
+      <c r="U32" t="s">
+        <v>87</v>
+      </c>
+      <c r="V32" t="s">
+        <v>88</v>
+      </c>
+      <c r="W32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A33" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>11740124</v>
+      </c>
+      <c r="D33">
+        <v>1174012</v>
+      </c>
+      <c r="E33">
+        <v>13.576000000000001</v>
+      </c>
+      <c r="F33">
+        <v>8.4489999999999996E-2</v>
+      </c>
+      <c r="G33" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1448482</v>
+      </c>
+      <c r="L33">
+        <v>1448482</v>
+      </c>
+      <c r="M33">
+        <v>14.861700000000001</v>
+      </c>
+      <c r="N33">
+        <v>1.042E-2</v>
+      </c>
+      <c r="O33" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="Q33" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="R33">
+        <v>10</v>
+      </c>
+      <c r="S33">
+        <v>11855637</v>
+      </c>
+      <c r="T33">
+        <v>1185564</v>
+      </c>
+      <c r="U33">
+        <v>13.5791</v>
+      </c>
+      <c r="V33">
+        <v>8.5319999999999993E-2</v>
+      </c>
+      <c r="W33" s="23">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A34" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1680829</v>
+      </c>
+      <c r="D34">
+        <v>1680829</v>
+      </c>
+      <c r="E34">
+        <v>19.436800000000002</v>
+      </c>
+      <c r="F34">
+        <v>1.21E-2</v>
+      </c>
+      <c r="G34" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>6034</v>
+      </c>
+      <c r="L34">
+        <v>6034</v>
+      </c>
+      <c r="M34">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="N34">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="O34">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="Q34" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1664733</v>
+      </c>
+      <c r="T34">
+        <v>1664733</v>
+      </c>
+      <c r="U34">
+        <v>19.067399999999999</v>
+      </c>
+      <c r="V34">
+        <v>1.1979999999999999E-2</v>
+      </c>
+      <c r="W34" s="23">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A35" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>633106</v>
+      </c>
+      <c r="D35">
+        <v>63311</v>
+      </c>
+      <c r="E35">
+        <v>0.73209999999999997</v>
+      </c>
+      <c r="F35">
+        <v>4.5599999999999998E-3</v>
+      </c>
+      <c r="G35">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J35">
+        <v>1394</v>
+      </c>
+      <c r="K35">
+        <v>135864728</v>
+      </c>
+      <c r="L35">
+        <v>97464</v>
+      </c>
+      <c r="N35">
+        <v>0.97775000000000001</v>
+      </c>
+      <c r="Q35" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="R35">
+        <v>8</v>
+      </c>
+      <c r="S35">
+        <v>5125902</v>
+      </c>
+      <c r="T35">
+        <v>640738</v>
+      </c>
+      <c r="U35">
+        <v>7.3388</v>
+      </c>
+      <c r="V35">
+        <v>3.6889999999999999E-2</v>
+      </c>
+      <c r="W35" s="23">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A36" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>20064</v>
+      </c>
+      <c r="D36">
+        <v>20064</v>
+      </c>
+      <c r="E36">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="F36">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="G36">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36">
+        <v>1397</v>
+      </c>
+      <c r="K36">
+        <v>138956340</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="R36">
+        <v>1378</v>
+      </c>
+      <c r="S36">
+        <v>120310068</v>
+      </c>
+      <c r="T36">
+        <v>87308</v>
+      </c>
+      <c r="V36">
+        <v>0.86580999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A37" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>5097492</v>
+      </c>
+      <c r="D37">
+        <v>637186</v>
+      </c>
+      <c r="E37">
+        <v>7.3682999999999996</v>
+      </c>
+      <c r="F37">
+        <v>3.6679999999999997E-2</v>
+      </c>
+      <c r="G37" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="Q37" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="R37">
+        <v>1397</v>
+      </c>
+      <c r="S37">
+        <v>138956340</v>
+      </c>
+      <c r="V37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A38" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>712198</v>
+      </c>
+      <c r="D38">
+        <v>89025</v>
+      </c>
+      <c r="E38">
+        <v>1.0295000000000001</v>
+      </c>
+      <c r="F38">
+        <v>5.13E-3</v>
+      </c>
+      <c r="G38">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A39" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39">
+        <v>1358</v>
+      </c>
+      <c r="C39">
+        <v>117435432</v>
+      </c>
+      <c r="D39">
+        <v>86477</v>
+      </c>
+      <c r="F39">
+        <v>0.84511999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A40" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40">
+        <v>1397</v>
+      </c>
+      <c r="C40">
+        <v>138956340</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE436C6-77C1-4035-9169-967A018712F0}">
+  <dimension ref="A1:W21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="Q6" s="21"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="27"/>
+      <c r="J7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q7" s="20"/>
+      <c r="R7" t="s">
+        <v>84</v>
+      </c>
+      <c r="S7" t="s">
+        <v>85</v>
+      </c>
+      <c r="T7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" t="s">
+        <v>87</v>
+      </c>
+      <c r="V7" t="s">
+        <v>88</v>
+      </c>
+      <c r="W7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2.42</v>
+      </c>
+      <c r="D8">
+        <v>2.4209999999999998</v>
+      </c>
+      <c r="E8">
+        <v>0.65468999999999999</v>
+      </c>
+      <c r="F8">
+        <v>1.2800000000000001E-3</v>
+      </c>
+      <c r="G8">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>258.72000000000003</v>
+      </c>
+      <c r="L8">
+        <v>43.12</v>
+      </c>
+      <c r="M8">
+        <v>13.366</v>
+      </c>
+      <c r="N8">
+        <v>0.13727</v>
+      </c>
+      <c r="O8" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>10.09</v>
+      </c>
+      <c r="T8">
+        <v>10.085800000000001</v>
+      </c>
+      <c r="U8">
+        <v>2.7385000000000002</v>
+      </c>
+      <c r="V8">
+        <v>5.3499999999999997E-3</v>
+      </c>
+      <c r="W8">
+        <v>9.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>509</v>
+      </c>
+      <c r="C9">
+        <v>1882.26</v>
+      </c>
+      <c r="D9">
+        <v>3.698</v>
+      </c>
+      <c r="F9">
+        <v>0.99872000000000005</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9">
+        <v>504</v>
+      </c>
+      <c r="K9">
+        <v>1625.96</v>
+      </c>
+      <c r="L9">
+        <v>3.226</v>
+      </c>
+      <c r="N9">
+        <v>0.86273</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="R9">
+        <v>509</v>
+      </c>
+      <c r="S9">
+        <v>1874.6</v>
+      </c>
+      <c r="T9">
+        <v>3.6829000000000001</v>
+      </c>
+      <c r="V9">
+        <v>0.99465000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10">
+        <v>510</v>
+      </c>
+      <c r="C10">
+        <v>1884.68</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10">
+        <v>510</v>
+      </c>
+      <c r="K10">
+        <v>1884.68</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="R10">
+        <v>510</v>
+      </c>
+      <c r="S10">
+        <v>1884.68</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="25"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="29"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.42</v>
+      </c>
+      <c r="D19">
+        <v>0.42009999999999997</v>
+      </c>
+      <c r="E19">
+        <v>0.11347</v>
+      </c>
+      <c r="F19">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="G19">
+        <v>0.73799999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20">
+        <v>509</v>
+      </c>
+      <c r="C20">
+        <v>1884.26</v>
+      </c>
+      <c r="D20">
+        <v>3.7019000000000002</v>
+      </c>
+      <c r="F20">
+        <v>0.99978</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21">
+        <v>510</v>
+      </c>
+      <c r="C21">
+        <v>1884.68</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>